<commit_message>
fixed the excel formulas.  added verification to a couple of the click Edit Header.
</commit_message>
<xml_diff>
--- a/Data/Input/TechnicalResultsTemplate.xlsx
+++ b/Data/Input/TechnicalResultsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/richard_king_uipath_com/Documents/Documents/Diamondback/OpenTicket_Audit/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="11_F25DC773A252ABDACC1048D9895C53825ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22BD7294-FD31-40BA-8DCF-67D0601A8529}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="11_F25DC773A252ABDACC1048D9895C53825ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DE14932-979C-44CC-A4FD-AF31F359E0AA}"/>
   <bookViews>
     <workbookView xWindow="-29100" yWindow="-7590" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -284,6 +284,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>331758</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78694837-9F54-ADBE-9B82-4B816E890EFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11207115" y="4343400"/>
+          <a:ext cx="3326418" cy="647756"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1809,8 +1858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FA38FB-2EF5-4767-8D99-2395F6EBE707}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2006,5 +2055,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>